<commit_message>
Add manual check feature with checkbox UI and fix delete button
- Implemented ManualCheck column in Excel database
- Added checkbox to UI for marking sites requiring manual check
- Migrated 10 hardcoded manual check sites to database
- Fixed delete button using event delegation instead of inline onclick
- Removed hardcoded cautionSites array from app.js
- Added comprehensive MANUAL_CHECK_FEATURE.md documentation
- Updated status logic to read manual check flag from backend
</commit_message>
<xml_diff>
--- a/data/name_and_urls.xlsx
+++ b/data/name_and_urls.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -409,6 +409,9 @@
       <c r="B1" t="str">
         <v>URL</v>
       </c>
+      <c r="C1" t="str">
+        <v>ManualCheck</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -417,6 +420,9 @@
       <c r="B2" t="str">
         <v>http://acwm.lacounty.gov</v>
       </c>
+      <c r="C2" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -425,6 +431,9 @@
       <c r="B3" t="str">
         <v>http://ad.lacounty.gov</v>
       </c>
+      <c r="C3" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -433,6 +442,9 @@
       <c r="B4" t="str">
         <v>http://auditor.lacounty.gov</v>
       </c>
+      <c r="C4" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -441,6 +453,9 @@
       <c r="B5" t="str">
         <v>http://wit.lacounty.gov</v>
       </c>
+      <c r="C5" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -449,6 +464,9 @@
       <c r="B6" t="str">
         <v>http://ccjv.lacounty.gov</v>
       </c>
+      <c r="C6" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -457,6 +475,9 @@
       <c r="B7" t="str">
         <v>https://isab.lacounty.gov/</v>
       </c>
+      <c r="C7" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -465,6 +486,9 @@
       <c r="B8" t="str">
         <v>http://khhoadirectory.lacounty.gov</v>
       </c>
+      <c r="C8" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -473,6 +497,9 @@
       <c r="B9" t="str">
         <v>http://redistricting.lacounty.gov</v>
       </c>
+      <c r="C9" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -481,6 +508,9 @@
       <c r="B10" t="str">
         <v>http://hildalsolis.org</v>
       </c>
+      <c r="C10" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -489,6 +519,9 @@
       <c r="B11" t="str">
         <v>https://mitchell.lacounty.gov/</v>
       </c>
+      <c r="C11" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -497,6 +530,9 @@
       <c r="B12" t="str">
         <v>http://lindseyhorvath.lacounty.gov</v>
       </c>
+      <c r="C12" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -505,6 +541,9 @@
       <c r="B13" t="str">
         <v>http://hahn.lacounty.gov</v>
       </c>
+      <c r="C13" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -513,6 +552,9 @@
       <c r="B14" t="str">
         <v>http://kathrynbarger.lacounty.gov</v>
       </c>
+      <c r="C14" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -521,6 +563,9 @@
       <c r="B15" t="str">
         <v>http://ceo.lacounty.gov</v>
       </c>
+      <c r="C15" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -529,6 +574,9 @@
       <c r="B16" t="str">
         <v>http://homeless.lacounty.gov</v>
       </c>
+      <c r="C16" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -537,6 +585,9 @@
       <c r="B17" t="str">
         <v>http://lacounty.gov</v>
       </c>
+      <c r="C17" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -545,6 +596,9 @@
       <c r="B18" t="str">
         <v>http://covid19.lacounty.gov</v>
       </c>
+      <c r="C18" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -553,6 +607,9 @@
       <c r="B19" t="str">
         <v>http://ready.lacounty.gov</v>
       </c>
+      <c r="C19" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -561,6 +618,9 @@
       <c r="B20" t="str">
         <v>http://ourcountyla.lacounty.gov</v>
       </c>
+      <c r="C20" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -569,6 +629,9 @@
       <c r="B21" t="str">
         <v>http://recovery.lacounty.gov</v>
       </c>
+      <c r="C21" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -577,6 +640,9 @@
       <c r="B22" t="str">
         <v>http://riskmanagement.lacounty.gov</v>
       </c>
+      <c r="C22" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -585,6 +651,9 @@
       <c r="B23" t="str">
         <v>http://cssd.lacounty.gov</v>
       </c>
+      <c r="C23" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -593,6 +662,9 @@
       <c r="B24" t="str">
         <v>http://animalcare.lacounty.gov</v>
       </c>
+      <c r="C24" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -601,6 +673,9 @@
       <c r="B25" t="str">
         <v>http://beaches.lacounty.gov</v>
       </c>
+      <c r="C25" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -609,6 +684,9 @@
       <c r="B26" t="str">
         <v>http://dcba.lacounty.gov</v>
       </c>
+      <c r="C26" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -617,6 +695,9 @@
       <c r="B27" t="str">
         <v>http://cares.lacounty.gov</v>
       </c>
+      <c r="C27" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -625,6 +706,9 @@
       <c r="B28" t="str">
         <v>http://oia.lacounty.gov</v>
       </c>
+      <c r="C28" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -633,6 +717,9 @@
       <c r="B29" t="str">
         <v>http://dcfs.lacounty.gov</v>
       </c>
+      <c r="C29" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -641,6 +728,9 @@
       <c r="B30" t="str">
         <v>https://layouthrights.com/</v>
       </c>
+      <c r="C30" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -649,6 +739,9 @@
       <c r="B31" t="str">
         <v>https://mylakids.dcfs.lacounty.gov/</v>
       </c>
+      <c r="C31" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -657,6 +750,9 @@
       <c r="B32" t="str">
         <v>http://dhs.lacounty.gov</v>
       </c>
+      <c r="C32" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -665,6 +761,9 @@
       <c r="B33" t="str">
         <v>http://dmh.lacounty.gov</v>
       </c>
+      <c r="C33" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -673,6 +772,9 @@
       <c r="B34" t="str">
         <v>https://www.deletethedivide.org/</v>
       </c>
+      <c r="C34" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -681,6 +783,9 @@
       <c r="B35" t="str">
         <v>http://childcare.lacounty.gov</v>
       </c>
+      <c r="C35" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -689,6 +794,9 @@
       <c r="B36" t="str">
         <v>https://ballonainterceptor.lacounty.gov/</v>
       </c>
+      <c r="C36" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -697,6 +805,9 @@
       <c r="B37" t="str">
         <v>https://calendar.pw.lacounty.gov/events/</v>
       </c>
+      <c r="C37" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -705,6 +816,9 @@
       <c r="B38" t="str">
         <v>https://cleanla.lacounty.gov/</v>
       </c>
+      <c r="C38" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -713,6 +827,9 @@
       <c r="B39" t="str">
         <v>http://content.pw.lacounty.gov</v>
       </c>
+      <c r="C39" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -721,6 +838,9 @@
       <c r="B40" t="str">
         <v>https://equity.pw.lacounty.gov/</v>
       </c>
+      <c r="C40" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -729,6 +849,9 @@
       <c r="B41" t="str">
         <v>https://infrastructurela.org/</v>
       </c>
+      <c r="C41" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -737,6 +860,9 @@
       <c r="B42" t="str">
         <v>https://ipm.lacounty.gov/</v>
       </c>
+      <c r="C42" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -745,6 +871,9 @@
       <c r="B43" t="str">
         <v>https://lowerlariver.org</v>
       </c>
+      <c r="C43" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -753,6 +882,9 @@
       <c r="B44" t="str">
         <v>https://oilandgas.lacounty.gov/</v>
       </c>
+      <c r="C44" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -761,6 +893,9 @@
       <c r="B45" t="str">
         <v>http://outreach.pw.lacounty.gov</v>
       </c>
+      <c r="C45" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -769,6 +904,9 @@
       <c r="B46" t="str">
         <v>https://waterforla.lacounty.gov/</v>
       </c>
+      <c r="C46" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -777,6 +915,9 @@
       <c r="B47" t="str">
         <v>https://lacountywomensleadership.org/</v>
       </c>
+      <c r="C47" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -785,6 +926,9 @@
       <c r="B48" t="str">
         <v>https://zerowaste.lacounty.gov/</v>
       </c>
+      <c r="C48" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -793,6 +937,9 @@
       <c r="B49" t="str">
         <v>http://dyd.lacounty.gov</v>
       </c>
+      <c r="C49" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -801,6 +948,9 @@
       <c r="B50" t="str">
         <v>https://emi.lacounty.gov/</v>
       </c>
+      <c r="C50" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -809,6 +959,9 @@
       <c r="B51" t="str">
         <v>http://fire.lacounty.gov</v>
       </c>
+      <c r="C51" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -817,6 +970,9 @@
       <c r="B52" t="str">
         <v>http://training.fire.lacounty.gov</v>
       </c>
+      <c r="C52" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -825,6 +981,9 @@
       <c r="B53" t="str">
         <v>https://fireiis.fire.lacounty.gov/</v>
       </c>
+      <c r="C53" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -833,6 +992,9 @@
       <c r="B54" t="str">
         <v>http://hr.lacounty.gov</v>
       </c>
+      <c r="C54" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -841,6 +1003,9 @@
       <c r="B55" t="str">
         <v>http://career-pathfinder.hr.lacounty.gov</v>
       </c>
+      <c r="C55" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -849,6 +1014,9 @@
       <c r="B56" t="str">
         <v>http://employee.hr.lacounty.gov</v>
       </c>
+      <c r="C56" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -857,6 +1025,9 @@
       <c r="B57" t="str">
         <v>http://isd.lacounty.gov</v>
       </c>
+      <c r="C57" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -865,6 +1036,9 @@
       <c r="B58" t="str">
         <v>http://egov.lacounty.gov</v>
       </c>
+      <c r="C58" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -873,6 +1047,9 @@
       <c r="B59" t="str">
         <v>http://isdtest.lacounty.gov</v>
       </c>
+      <c r="C59" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -881,6 +1058,9 @@
       <c r="B60" t="str">
         <v>http://rideshare.lacounty.gov</v>
       </c>
+      <c r="C60" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -889,6 +1069,9 @@
       <c r="B61" t="str">
         <v>http://wppro.lacounty.gov</v>
       </c>
+      <c r="C61" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -897,6 +1080,9 @@
       <c r="B62" t="str">
         <v>http://central.gis.lacounty.gov</v>
       </c>
+      <c r="C62" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -905,6 +1091,9 @@
       <c r="B63" t="str">
         <v>http://doingbusiness.lacounty.gov</v>
       </c>
+      <c r="C63" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -913,6 +1102,9 @@
       <c r="B64" t="str">
         <v>http://dc1.lacounty.gov</v>
       </c>
+      <c r="C64" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -921,6 +1113,9 @@
       <c r="B65" t="str">
         <v>http://procurement.lacounty.gov</v>
       </c>
+      <c r="C65" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -929,6 +1124,9 @@
       <c r="B66" t="str">
         <v>http://jcod.lacounty.gov</v>
       </c>
+      <c r="C66" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -937,6 +1135,9 @@
       <c r="B67" t="str">
         <v>https://justiceconnect.org/</v>
       </c>
+      <c r="C67" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -945,6 +1146,9 @@
       <c r="B68" t="str">
         <v>https://lacountyparkneeds.org/</v>
       </c>
+      <c r="C68" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -953,6 +1157,9 @@
       <c r="B69" t="str">
         <v>http://lanaic.lacounty.gov</v>
       </c>
+      <c r="C69" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -961,6 +1168,9 @@
       <c r="B70" t="str">
         <v>http://grac.lacounty.gov</v>
       </c>
+      <c r="C70" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -969,6 +1179,9 @@
       <c r="B71" t="str">
         <v>http://lacountylibrary.org</v>
       </c>
+      <c r="C71" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -977,6 +1190,9 @@
       <c r="B72" t="str">
         <v>http://me.lacounty.gov</v>
       </c>
+      <c r="C72" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -985,6 +1201,9 @@
       <c r="B73" t="str">
         <v>http://mva.lacounty.gov</v>
       </c>
+      <c r="C73" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -993,6 +1212,9 @@
       <c r="B74" t="str">
         <v>http://my.lacounty.gov</v>
       </c>
+      <c r="C74" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1001,6 +1223,9 @@
       <c r="B75" t="str">
         <v>https://mywdacs.lacounty.gov/</v>
       </c>
+      <c r="C75" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1009,6 +1234,9 @@
       <c r="B76" t="str">
         <v>https://opportunity.lacounty.gov/</v>
       </c>
+      <c r="C76" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1017,6 +1245,9 @@
       <c r="B77" t="str">
         <v>http://parks.lacounty.gov</v>
       </c>
+      <c r="C77" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1025,6 +1256,9 @@
       <c r="B78" t="str">
         <v>http://rposd.lacounty.gov</v>
       </c>
+      <c r="C78" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1033,6 +1267,9 @@
       <c r="B79" t="str">
         <v xml:space="preserve">https://permits.lacounty.gov/ </v>
       </c>
+      <c r="C79" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1041,6 +1278,9 @@
       <c r="B80" t="str">
         <v>http://probation.lacounty.gov</v>
       </c>
+      <c r="C80" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1049,6 +1289,9 @@
       <c r="B81" t="str">
         <v>http://pubdef.lacounty.gov</v>
       </c>
+      <c r="C81" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1057,6 +1300,9 @@
       <c r="B82" t="str">
         <v>http://apd.lacounty.gov</v>
       </c>
+      <c r="C82" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1065,6 +1311,9 @@
       <c r="B83" t="str">
         <v>http://pdportal.lacounty.gov</v>
       </c>
+      <c r="C83" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1073,6 +1322,9 @@
       <c r="B84" t="str">
         <v>http://idco.lacounty.gov</v>
       </c>
+      <c r="C84" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1081,18 +1333,13 @@
       <c r="B85" t="str">
         <v>https://ttc.lacounty.gov/</v>
       </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>Ctep</v>
-      </c>
-      <c r="B86" t="str">
-        <v>http://ctep-dev.wppro.lacounty.gov/</v>
+      <c r="C85" t="str">
+        <v>No</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B86"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C85"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>